<commit_message>
updated examples to use Data oject
</commit_message>
<xml_diff>
--- a/examples/HEAT/JAIS_2023/BERTopic_model_results/SAFECOM_Hazards_v2.xlsx
+++ b/examples/HEAT/JAIS_2023/BERTopic_model_results/SAFECOM_Hazards_v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srandrad\smart_nlp\results\SAFECOM_hazards\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srandrad\smart_nlp\examples\HEAT\JAIS_2023\BERTopic_model_results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDBFE5F9-DB9C-40DF-A99C-2E40D69B0AB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68C1B422-2DFE-4A09-8A3D-9A5462C65B0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="3240" yWindow="3240" windowWidth="17280" windowHeight="10044" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="topic-focused" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="78">
   <si>
     <t>Topic Number</t>
   </si>
@@ -262,6 +262,9 @@
   </si>
   <si>
     <t>incursion, intrusion, conflict</t>
+  </si>
+  <si>
+    <t>Dropped Load</t>
   </si>
 </sst>
 </file>
@@ -632,7 +635,7 @@
   <dimension ref="A1:R26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -961,6 +964,9 @@
       </c>
       <c r="E25" t="s">
         <v>66</v>
+      </c>
+      <c r="R25" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.3">
@@ -987,15 +993,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BE83D2F83C1FDB48876C470B698CB487" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bce9e4f6f075ed410398444cb9137584">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e7ec8b44-adb9-4117-b85f-c094036dda67" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7788eebe476cdd7e70505f9cfa3bf5bb" ns2:_="">
     <xsd:import namespace="e7ec8b44-adb9-4117-b85f-c094036dda67"/>
@@ -1159,6 +1156,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1166,14 +1172,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A778DB98-8470-4BE2-BC19-F7530CBE547A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{68C50802-5E8D-47AA-9FDE-9192ABDA8BD3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1187,6 +1185,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A778DB98-8470-4BE2-BC19-F7530CBE547A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>